<commit_message>
protected sheets with PW: Ingenion
</commit_message>
<xml_diff>
--- a/docs/_static/tvs3_io_planning.xlsx
+++ b/docs/_static/tvs3_io_planning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omarhaddad/Library/CloudStorage/Dropbox/Mac/Documents/GitHub_Ingenion/tvs3docs/docs/_static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4321C063-2738-2E4B-9EAD-33814D9CF085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF01054E-B4B8-0D42-8646-4B6F11A2955F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26360" yWindow="-6120" windowWidth="37460" windowHeight="15400" activeTab="4" xr2:uid="{90D22351-47D1-C64B-9C15-8092C2A0903E}"/>
+    <workbookView xWindow="26360" yWindow="-6120" windowWidth="37460" windowHeight="15400" activeTab="8" xr2:uid="{90D22351-47D1-C64B-9C15-8092C2A0903E}"/>
   </bookViews>
   <sheets>
     <sheet name="FPGA IO" sheetId="1" r:id="rId1"/>
@@ -12918,6 +12918,7 @@
       <c r="L220" s="1"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="BmGmOGKbITJOHatQ1cS2rO8H+NnCJbI3X1ru8oxgMbu7/rPaqVjGleRWum3v1wwKZKkI/UzR/PGp/xBsRQUtCA==" saltValue="4VrO+ezHSfHQfFPV2hORcw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
@@ -14266,6 +14267,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="NLix5dHSF33jfnSSnuuMB79CT3ItuMPXxUdG8sroFNiW+ylSONAmw/qQ2ib2nzq9lqBnaud+GIcjfrhw7KGEcg==" saltValue="/S7SakNvJ+Gy3is/ihWsLg==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -15611,7 +15613,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="DzF+HSt3IZwEp7hVgxg7P4c7osUFX4UEOcWw7hZmr7b9wdmuSIYPQqH+vUhRJK7av5XIOQFYD/lG5WYLOM1/dQ==" saltValue="+c+UNYhm5DSVJgKEppAlCA==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -16959,7 +16961,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="I2UPGRFSGry+VE2ShPext8Blp4CSB5kz+wxlBWJR6mVljw65hu7eb0JtrSDgk6YcWP37ZpaxXYVkutKCrRLeCw==" saltValue="EalbW/LRH2dndfFqqqS/1A==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -16971,7 +16973,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{745DD610-88AD-0240-AE5E-E5757E0EAF7D}">
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+    <sheetView zoomScale="125" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -19655,7 +19657,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="baaM6k7Q83Av6Is6vkdknRdCYYxvvdmZFCshDg40IKHKwRTiNsTYqg79KhKa88Zmp4HGps94x8JiI9oFIDZkyw==" saltValue="whSnGS8nKmK7J1IiB6Wj8w==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -20556,7 +20558,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="SDefwrm62x6o+SsiiGEK34W7qTLqVNgrcbI1B9/ISl9vtrKGb0IYWyBb0fdfr2gDdypyW/nK7YnxPv/zo03WtQ==" saltValue="kj/C3KyEQDO3zSA1BmOhAQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -21824,7 +21826,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dkkgS+av9wTD9Yl9VHMntWkWGew0I4WXd0Nj6/KGXMbj20BCL6zbgbIvkSI0lXNsI9m08ngS2QZi/z+Rb+LI6Q==" saltValue="a8uwPlmIo0v/Wc9XB403Og==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -21836,8 +21838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E0DF3CA-3C09-684A-9446-F52B23446FF5}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22457,7 +22459,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="VVhDfeP/anK1k649/HXbSC6pgC0L6v87h5Wk8RKgaAyVF8vIJLMt9D4yRGx8KJvojwFL0zQdzkUS9g83D5Wh3w==" saltValue="aVX9+GJgfjlElyvZ8QMK6A==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>